<commit_message>
temp update for weekend
</commit_message>
<xml_diff>
--- a/issue tracking-2019.xlsx
+++ b/issue tracking-2019.xlsx
@@ -1,27 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weifan\Documents\CM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6883A884-F826-49DE-9AF3-1D651FF31F8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28245" windowHeight="12465" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019-4-6" sheetId="12" r:id="rId1"/>
     <sheet name="2019-4-9" sheetId="13" r:id="rId2"/>
     <sheet name="2019-4-10" sheetId="14" r:id="rId3"/>
     <sheet name="2019-4-11" sheetId="15" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2019-4-10'!$A$1:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2019-4-9'!$A$1:$G$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2019-4-10'!$A$1:$G$10</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
   <si>
     <t>序号</t>
   </si>
@@ -162,7 +169,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -172,7 +179,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -227,29 +234,65 @@
   <si>
     <t>7,8和9,10课程显示也分开。</t>
   </si>
+  <si>
+    <t>更改了老师申报的强制要求检查。难度9要求至少1门，难度7和9的总数要求至少5门，总数至少7门。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码在阿里云的机器上。D:\FuDan\debug\CM-master\CM-master</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>课程的编辑框，里面的数据和数据库读出写入的位置没有对好。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>open</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>课程列表显示代码，最后一列平行课漏掉了，导致显示出错。（就是我们中午解决的那个）</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>课程编辑窗口里没有可以把课程设置成非激活状态的地方。修改激活状态，修改平行课数，修改老师数，修改可选教师列表，这些都经常用到。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>我在workbench里面把某课程设为非激活状态。期望的结果是在课程管理页面仍旧可以看到这门课程，状态是非激活，在教师管理页面的教师个人中不能看到这门非激活课程。实际结果是，在课程管理页面里，默认load这个页面的时候，显示正确，但是当在左侧导航栏选择过学科组再提交之后，就不能看到这门课程了，而且其他显示课程的”状态“显示“0”，“平行课数”的数字显示位置也有点太靠左，反正就是怪怪的，但是不管怎样，此处应该还是能够看到非激活课程。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>open</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入的老师信息，老师年龄不正确，年份都+4了，月份没错，日+1。这个会影响排课结果。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>日期转换的模式选错了。</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -262,156 +305,26 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
+      <sz val="9"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,194 +349,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -631,255 +358,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -952,62 +437,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1265,29 +718,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="5.6328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="53.625" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="8.875" customWidth="1"/>
-    <col min="7" max="7" width="65.25" customWidth="1"/>
+    <col min="3" max="3" width="53.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="6" max="6" width="8.90625" customWidth="1"/>
+    <col min="7" max="7" width="65.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1313,7 +765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="28.5" spans="1:7">
+    <row r="2" spans="1:7" ht="29">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1329,7 +781,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" ht="57" spans="1:7">
+    <row r="3" spans="1:7" ht="58">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1347,36 +799,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
+    <row r="4" spans="1:7">
       <c r="C4" s="22"/>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="1:7">
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="1:7">
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="1:7">
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="G7" s="23"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -1384,14 +836,14 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.25" customWidth="1"/>
-    <col min="2" max="2" width="9.125" customWidth="1"/>
-    <col min="3" max="3" width="38.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.375" customWidth="1"/>
+    <col min="1" max="1" width="7.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="3" width="38.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.36328125" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="78.25" style="3" customWidth="1"/>
+    <col min="7" max="7" width="78.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1417,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="42.75" hidden="1" spans="1:6">
+    <row r="2" spans="1:7" ht="43.5" hidden="1">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1437,7 +889,7 @@
         <v>43564</v>
       </c>
     </row>
-    <row r="3" ht="57" hidden="1" spans="1:7">
+    <row r="3" spans="1:7" ht="72.5" hidden="1">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1460,7 +912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" ht="42.75" hidden="1" spans="1:7">
+    <row r="4" spans="1:7" ht="43.5" hidden="1">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1483,7 +935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" ht="28.5" spans="1:7">
+    <row r="5" spans="1:7" ht="43.5">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1503,7 +955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" ht="42.75" hidden="1" spans="1:7">
+    <row r="6" spans="1:7" ht="43.5" hidden="1">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1526,7 +978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" ht="71.25" hidden="1" spans="1:7">
+    <row r="7" spans="1:7" ht="72.5" hidden="1">
       <c r="A7">
         <v>8</v>
       </c>
@@ -1549,7 +1001,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" ht="42.75" hidden="1" spans="1:7">
+    <row r="8" spans="1:7" ht="43.5" hidden="1">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1572,7 +1024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="42.75" spans="1:7">
+    <row r="9" spans="1:7" ht="43.5">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1595,7 +1047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" ht="71.25" spans="1:5">
+    <row r="10" spans="1:7" ht="72.5">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1612,7 +1064,7 @@
         <v>43564</v>
       </c>
     </row>
-    <row r="11" ht="57" spans="1:7">
+    <row r="11" spans="1:7" ht="72.5">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1632,7 +1084,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" ht="85.5" hidden="1" spans="1:7">
+    <row r="12" spans="1:7" ht="101.5" hidden="1">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1655,7 +1107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" ht="57" hidden="1" spans="1:7">
+    <row r="13" spans="1:7" ht="58" hidden="1">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1678,7 +1130,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" ht="42.75" spans="1:7">
+    <row r="14" spans="1:7" ht="43.5">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1698,7 +1150,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" ht="28.5" hidden="1" spans="1:7">
+    <row r="15" spans="1:7" ht="29" hidden="1">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1721,7 +1173,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" ht="57" spans="1:7">
+    <row r="16" spans="1:7" ht="72.5">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1742,39 +1194,38 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G16">
+  <autoFilter ref="A1:G16" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="equal" val="open"/>
-        <customFilter operator="equal" val="re-open"/>
-      </customFilters>
+      <filters>
+        <filter val="open"/>
+        <filter val="re-open"/>
+      </filters>
     </filterColumn>
-    <extLst/>
   </autoFilter>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:G$1048576"/>
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.125" customWidth="1"/>
-    <col min="2" max="2" width="9.125" customWidth="1"/>
-    <col min="3" max="3" width="36.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="74.25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="3" width="36.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="6" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="74.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1800,7 +1251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="85.5" spans="1:6">
+    <row r="2" spans="1:7" ht="87">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1820,7 +1271,7 @@
         <v>43565</v>
       </c>
     </row>
-    <row r="3" ht="42.75" spans="1:6">
+    <row r="3" spans="1:7" ht="43.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1840,7 +1291,7 @@
         <v>43565</v>
       </c>
     </row>
-    <row r="4" ht="85.5" spans="1:6">
+    <row r="4" spans="1:7" ht="87">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1858,7 +1309,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" ht="42.75" spans="1:6">
+    <row r="5" spans="1:7" ht="43.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1878,7 +1329,7 @@
         <v>43565</v>
       </c>
     </row>
-    <row r="6" ht="28.5" spans="1:7">
+    <row r="6" spans="1:7" ht="29">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1901,7 +1352,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" ht="42.75" spans="1:7">
+    <row r="7" spans="1:7" ht="58">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1920,7 +1371,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" ht="28.5" spans="1:6">
+    <row r="8" spans="1:7" ht="29">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1940,7 +1391,7 @@
         <v>43565</v>
       </c>
     </row>
-    <row r="9" s="14" customFormat="1" ht="28.5" spans="1:7">
+    <row r="9" spans="1:7" s="14" customFormat="1" ht="29">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -1963,7 +1414,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" ht="28.5" spans="1:5">
+    <row r="10" spans="1:7" ht="43.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1980,67 +1431,64 @@
         <v>43565</v>
       </c>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="1:7">
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="19"/>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="1:7">
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="3:6">
+    <row r="13" spans="1:7">
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="3:5">
+    <row r="14" spans="1:7">
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="3:6">
+    <row r="15" spans="1:7">
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="3:5">
+    <row r="16" spans="1:7">
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G10">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <autoFilter ref="A1:G10" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.125" customWidth="1"/>
-    <col min="2" max="2" width="9.125" customWidth="1"/>
-    <col min="3" max="3" width="36.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="74.25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="3" width="36.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="6" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="74.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2066,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="128.25" spans="1:7">
+    <row r="2" spans="1:7" ht="130.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2089,7 +1537,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="99.75" spans="1:7">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="101.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2108,7 +1556,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" ht="28.5" spans="1:7">
+    <row r="4" spans="1:7" ht="29">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2131,7 +1579,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" ht="42.75" spans="1:6">
+    <row r="5" spans="1:7" ht="58">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2149,7 +1597,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" ht="28.5" spans="1:6">
+    <row r="6" spans="1:7" ht="29">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2167,7 +1615,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" ht="28.5" spans="1:7">
+    <row r="7" spans="1:7" ht="29">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -2190,19 +1638,187 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="3:6">
+    <row r="8" spans="1:7">
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="1:7">
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C2B82B-3298-422C-B142-DB336E683DEC}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="7.08984375" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="3" max="3" width="36.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="6" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="74.26953125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="43.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="6">
+        <v>43567</v>
+      </c>
+      <c r="F2" s="6">
+        <v>43567</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="6">
+        <v>43567</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="6">
+        <v>43567</v>
+      </c>
+      <c r="F4" s="6">
+        <v>43568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="58">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="6">
+        <v>43567</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="188.5">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="6">
+        <v>43567</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.5">
+      <c r="A7" s="25">
+        <v>1</v>
+      </c>
+      <c r="B7" s="25">
+        <v>1</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="27">
+        <v>43567</v>
+      </c>
+      <c r="F7" s="6">
+        <v>43568</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug for 2019-4-18
</commit_message>
<xml_diff>
--- a/issue tracking-2019.xlsx
+++ b/issue tracking-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28245" windowHeight="12465" activeTab="4"/>
+    <workbookView windowWidth="28245" windowHeight="12465" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2019-4-6" sheetId="12" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="2019-4-10" sheetId="14" r:id="rId3"/>
     <sheet name="2019-4-11" sheetId="15" r:id="rId4"/>
     <sheet name="2019-4-12" sheetId="16" r:id="rId5"/>
+    <sheet name="2019-4-18" sheetId="17" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2019-4-9'!$A$1:$G$16</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
   <si>
     <t>序号</t>
   </si>
@@ -249,6 +250,39 @@
   <si>
     <t>日期转换的模式选错了。</t>
   </si>
+  <si>
+    <t>课程管理页面，教师数编辑失败</t>
+  </si>
+  <si>
+    <t>18/4/2019</t>
+  </si>
+  <si>
+    <t>默认课程计划非激活如果为空保存编辑信息都会失败。增加空的处理</t>
+  </si>
+  <si>
+    <t>改了激活状态提交后，数据库里面的必修选修没了</t>
+  </si>
+  <si>
+    <t>18/4/2020</t>
+  </si>
+  <si>
+    <t>在第一天修改完之后并没有出现。根据代码如果激活状态为空应该是没法体检编辑的才对</t>
+  </si>
+  <si>
+    <t>教师信息管理中，教务员看不到非激活老师</t>
+  </si>
+  <si>
+    <t>18/4/2021</t>
+  </si>
+  <si>
+    <t>加入非激活老师数。但是其他统计都不算上</t>
+  </si>
+  <si>
+    <t>微调可以修改老师，同步更新工作量</t>
+  </si>
+  <si>
+    <t>18/4/2022</t>
+  </si>
 </sst>
 </file>
 
@@ -256,11 +290,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,14 +317,50 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,61 +374,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,6 +398,22 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -388,38 +422,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -432,6 +444,21 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -460,31 +487,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,151 +667,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,15 +678,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -687,6 +705,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -698,26 +736,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -751,6 +769,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -759,10 +786,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -771,146 +798,143 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -920,12 +944,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -969,9 +996,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1345,8 +1369,8 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5">
+      <c r="D2" s="3"/>
+      <c r="E2" s="4">
         <v>43562</v>
       </c>
       <c r="G2" s="1"/>
@@ -1361,8 +1385,8 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5">
+      <c r="D3" s="3"/>
+      <c r="E3" s="4">
         <v>43563</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1371,25 +1395,25 @@
     </row>
     <row r="4" spans="3:5">
       <c r="C4" s="22"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="3:5">
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="3:7">
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="G6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="3:7">
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="G7" s="23"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1413,7 +1437,7 @@
     <col min="3" max="3" width="38.725" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.36666666666667" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="78.2666666666667" style="2" customWidth="1"/>
+    <col min="7" max="7" width="78.2666666666667" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1446,16 +1470,16 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>43564</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>43564</v>
       </c>
     </row>
@@ -1469,16 +1493,16 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>43564</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>43564</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1492,16 +1516,16 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>43564</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>43564</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1512,13 +1536,13 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>43564</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -1535,16 +1559,16 @@
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>43564</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>43564</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1558,16 +1582,16 @@
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>43564</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>43564</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1581,16 +1605,16 @@
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>43564</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>43564</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1607,10 +1631,10 @@
       <c r="D9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>43564</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>43564</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -1624,13 +1648,13 @@
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>43564</v>
       </c>
     </row>
@@ -1641,10 +1665,10 @@
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="9">
@@ -1661,10 +1685,10 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="9">
@@ -1684,19 +1708,19 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>43564</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>43564</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1707,16 +1731,16 @@
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>43564</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1727,19 +1751,19 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>43564</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>43564</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1750,16 +1774,16 @@
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>43564</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1796,7 +1820,7 @@
     <col min="3" max="3" width="36.0916666666667" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.09166666666667" customWidth="1"/>
     <col min="5" max="6" width="11.0916666666667" customWidth="1"/>
-    <col min="7" max="7" width="74.2666666666667" style="2" customWidth="1"/>
+    <col min="7" max="7" width="74.2666666666667" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1829,16 +1853,16 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>43565</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>43565</v>
       </c>
     </row>
@@ -1849,16 +1873,16 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>43565</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>43565</v>
       </c>
     </row>
@@ -1869,16 +1893,16 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>43565</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" ht="42.75" spans="1:6">
       <c r="A5">
@@ -1887,16 +1911,16 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>43565</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>43565</v>
       </c>
     </row>
@@ -1907,19 +1931,19 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>43565</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>43565</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1930,17 +1954,17 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>43565</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" ht="28.5" spans="1:6">
       <c r="A8">
@@ -1949,16 +1973,16 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>43565</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>43565</v>
       </c>
     </row>
@@ -1992,50 +2016,50 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>43565</v>
       </c>
     </row>
     <row r="11" spans="3:7">
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="9"/>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="3:7">
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="3:6">
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="3:5">
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="3:6">
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="3:5">
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G10">
@@ -2062,7 +2086,7 @@
     <col min="3" max="3" width="36.0916666666667" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.09166666666667" customWidth="1"/>
     <col min="5" max="6" width="11.0916666666667" customWidth="1"/>
-    <col min="7" max="7" width="74.2666666666667" style="2" customWidth="1"/>
+    <col min="7" max="7" width="74.2666666666667" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2095,33 +2119,33 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>43566</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>43566</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="1" ht="99.75" spans="1:7">
-      <c r="A3" s="4">
+    <row r="3" s="3" customFormat="1" ht="99.75" spans="1:7">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="9">
@@ -2137,19 +2161,19 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>43566</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>43566</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2160,16 +2184,16 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>43566</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" ht="28.5" spans="1:6">
       <c r="A6">
@@ -2178,16 +2202,16 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>43566</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" ht="28.5" spans="1:7">
       <c r="A7" s="12">
@@ -2205,23 +2229,23 @@
       <c r="E7" s="15">
         <v>43566</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>43566</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="3:6">
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="3:5">
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2234,8 +2258,8 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -2245,7 +2269,7 @@
     <col min="3" max="3" width="36.0916666666667" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.09166666666667" customWidth="1"/>
     <col min="5" max="6" width="11.0916666666667" customWidth="1"/>
-    <col min="7" max="7" width="74.2666666666667" style="2" customWidth="1"/>
+    <col min="7" max="7" width="74.2666666666667" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2278,19 +2302,19 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>43567</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>43567</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2307,10 +2331,10 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>43567</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>43569</v>
       </c>
     </row>
@@ -2327,10 +2351,10 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>43567</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>43568</v>
       </c>
     </row>
@@ -2347,10 +2371,10 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>43567</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>43569</v>
       </c>
     </row>
@@ -2367,33 +2391,33 @@
       <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>43567</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>43569</v>
       </c>
     </row>
     <row r="7" ht="42.75" spans="1:7">
-      <c r="A7" s="6">
-        <v>1</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="8">
         <v>43567</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>43568</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2402,4 +2426,156 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="4" max="4" width="5.625" customWidth="1"/>
+    <col min="5" max="6" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="85.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" ht="28.5" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" ht="28.5" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" ht="28.5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" s="1"/>
+      <c r="D6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>